<commit_message>
add column status to enable/disable services
</commit_message>
<xml_diff>
--- a/mappa-servizi.xlsx
+++ b/mappa-servizi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t xml:space="preserve">Service Type</t>
   </si>
@@ -43,10 +43,13 @@
     <t xml:space="preserve">Reject</t>
   </si>
   <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
   </si>
   <si>
     <t xml:space="preserve">HTTP</t>
@@ -55,24 +58,30 @@
     <t xml:space="preserve">s1.rivetweb.org</t>
   </si>
   <si>
+    <t xml:space="preserve">shorter.rivetweb.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pastorious.rivetweb.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disable</t>
+  </si>
+  <si>
     <t xml:space="preserve">192.168.244.216</t>
   </si>
   <si>
-    <t xml:space="preserve">IT ES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shorter.rivetweb.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pastorious.rivetweb.org</t>
-  </si>
-  <si>
     <t xml:space="preserve">IT</t>
   </si>
   <si>
@@ -82,10 +91,10 @@
     <t xml:space="preserve">s2.rivetweb.org</t>
   </si>
   <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
     <t xml:space="preserve">192.168.244.217</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT</t>
   </si>
 </sst>
 </file>
@@ -296,13 +305,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.69"/>
@@ -311,7 +320,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,157 +345,181 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>443</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2222</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2223</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>5432</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>5411</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>443</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>80</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2224</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>5433</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>5411</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reformatting some rule, change frontends name definition, reorder columns is test datasheet
</commit_message>
<xml_diff>
--- a/mappa-servizi.xlsx
+++ b/mappa-servizi.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">Service Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Port</t>
+  </si>
+  <si>
     <t xml:space="preserve">SNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port</t>
   </si>
   <si>
     <t xml:space="preserve">Target IP</t>
@@ -308,14 +308,14 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.79"/>
@@ -359,11 +359,11 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>443</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -385,7 +385,7 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="B3" s="1" t="n">
         <v>2222</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -408,7 +408,7 @@
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="B4" s="1" t="n">
         <v>2223</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -431,7 +431,7 @@
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="B5" s="1" t="n">
         <v>5432</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -454,11 +454,11 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>443</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>17</v>
@@ -480,7 +480,7 @@
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="B7" s="1" t="n">
         <v>2224</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -503,7 +503,7 @@
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="B8" s="1" t="n">
         <v>5433</v>
       </c>
       <c r="D8" s="1" t="s">

</xml_diff>

<commit_message>
now producing a correct configuration file
</commit_message>
<xml_diff>
--- a/mappa-servizi.xlsx
+++ b/mappa-servizi.xlsx
@@ -76,13 +76,13 @@
     <t xml:space="preserve">pastorious.rivetweb.org</t>
   </si>
   <si>
+    <t xml:space="preserve">192.168.244.216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
     <t xml:space="preserve">disable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192.168.244.216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT</t>
   </si>
   <si>
     <t xml:space="preserve">PGSQL</t>
@@ -308,13 +308,13 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.99"/>
@@ -401,7 +401,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -412,19 +412,19 @@
         <v>2223</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,19 +435,19 @@
         <v>5432</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>5411</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +496,7 @@
         <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,7 +519,7 @@
         <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more efficient acl determination and grouping
</commit_message>
<xml_diff>
--- a/mappa-servizi.xlsx
+++ b/mappa-servizi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t xml:space="preserve">Service Type</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">shorter.rivetweb.org</t>
   </si>
   <si>
-    <t xml:space="preserve">IT ES</t>
+    <t xml:space="preserve">IT US</t>
   </si>
   <si>
     <t xml:space="preserve">ALL</t>
@@ -70,12 +70,12 @@
     <t xml:space="preserve">enable</t>
   </si>
   <si>
+    <t xml:space="preserve">pastorious.rivetweb.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">SSH</t>
   </si>
   <si>
-    <t xml:space="preserve">pastorious.rivetweb.org</t>
-  </si>
-  <si>
     <t xml:space="preserve">192.168.244.216</t>
   </si>
   <si>
@@ -91,10 +91,13 @@
     <t xml:space="preserve">s2.rivetweb.org</t>
   </si>
   <si>
+    <t xml:space="preserve">167.172.169.214 RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.244.217</t>
+  </si>
+  <si>
     <t xml:space="preserve">PT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192.168.244.217</t>
   </si>
 </sst>
 </file>
@@ -305,10 +308,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -319,7 +322,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.93"/>
   </cols>
   <sheetData>
@@ -383,19 +386,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2222</v>
+        <v>443</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
@@ -406,39 +412,39 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>5432</v>
+        <v>2223</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>5411</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>19</v>
@@ -452,73 +458,96 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>443</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>5432</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>80</v>
+        <v>5411</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>2224</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" s="1" t="n">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>5433</v>
+        <v>2224</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>5433</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="n">
         <v>5411</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first complete and working configuration automatically generated
</commit_message>
<xml_diff>
--- a/mappa-servizi.xlsx
+++ b/mappa-servizi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t xml:space="preserve">Service Type</t>
   </si>
@@ -70,25 +70,28 @@
     <t xml:space="preserve">enable</t>
   </si>
   <si>
+    <t xml:space="preserve">164.92.216.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.244.216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PGSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s2.rivetweb.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">pastorious.rivetweb.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192.168.244.216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PGSQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s2.rivetweb.org</t>
   </si>
   <si>
     <t xml:space="preserve">167.172.169.214 RU</t>
@@ -311,10 +314,10 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.12"/>
@@ -490,7 +493,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>80</v>
@@ -499,7 +502,7 @@
         <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>15</v>
@@ -513,13 +516,13 @@
         <v>2224</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -536,13 +539,13 @@
         <v>5433</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>5411</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
first working release with sub-optimal ACL generation though
</commit_message>
<xml_diff>
--- a/mappa-servizi.xlsx
+++ b/mappa-servizi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t xml:space="preserve">Service Type</t>
   </si>
@@ -64,34 +64,37 @@
     <t xml:space="preserve">IT US</t>
   </si>
   <si>
+    <t xml:space="preserve">rogue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">164.92.216.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.244.216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PGSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s2.rivetweb.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pastorious.rivetweb.org</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">164.92.216.90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192.168.244.216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PGSQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s2.rivetweb.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pastorious.rivetweb.org</t>
   </si>
   <si>
     <t xml:space="preserve">167.172.169.214 RU</t>
@@ -314,7 +317,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -325,7 +328,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="37.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.93"/>
   </cols>
   <sheetData>
@@ -406,9 +410,6 @@
       <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
@@ -429,9 +430,6 @@
       <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
@@ -452,9 +450,6 @@
       <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
@@ -475,11 +470,8 @@
       <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,10 +491,10 @@
         <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>15</v>
@@ -516,19 +508,16 @@
         <v>2224</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,16 +528,13 @@
         <v>5433</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>5411</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>20</v>

</xml_diff>